<commit_message>
agregue el whatsapp en editar trabajo
</commit_message>
<xml_diff>
--- a/dist/Sistema CPIM/registros.xlsx
+++ b/dist/Sistema CPIM/registros.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X96"/>
+  <dimension ref="A1:X98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A95" sqref="A95"/>
@@ -8260,21 +8260,6 @@
           <t>218000</t>
         </is>
       </c>
-      <c r="N87" t="inlineStr">
-        <is>
-          <t>40000</t>
-        </is>
-      </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>48000</t>
-        </is>
-      </c>
-      <c r="P87" t="inlineStr">
-        <is>
-          <t>48000</t>
-        </is>
-      </c>
       <c r="R87" t="inlineStr">
         <is>
           <t>No pagado</t>
@@ -8896,6 +8881,151 @@
       <c r="X96" s="5" t="inlineStr">
         <is>
           <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\OBRA NUEVA\FARIAS OSVALDO\FARIAS LUCIANO OSVALDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>05/06/2025</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>MMO</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Digital</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Obra nueva</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>CORDOVES MAURO IVAN</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>BUSTOS KARINA VANESSA</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>CALLE (47) M. HERRERA N° 4907</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>34987/2024</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>4072</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>22090</t>
+        </is>
+      </c>
+      <c r="R97" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="X97" t="inlineStr">
+        <is>
+          <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\OBRA NUEVA\CORDOVES MAURO IVAN\BUSTOS KARINA VANESSA</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>06/06/2025</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Ingeniero</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Digital</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Registración</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>EDSBERG IVAN</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>CORTES MARIA DANIELLA</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>Lanusse N° 2072</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>15492/M/1996</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>4574</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>16465</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr"/>
+      <c r="N98" t="inlineStr"/>
+      <c r="O98" t="inlineStr"/>
+      <c r="P98" t="inlineStr"/>
+      <c r="Q98" t="inlineStr"/>
+      <c r="R98" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="S98" t="inlineStr">
+        <is>
+          <t>No pagado</t>
+        </is>
+      </c>
+      <c r="T98" t="inlineStr"/>
+      <c r="U98" t="inlineStr"/>
+      <c r="V98" t="inlineStr"/>
+      <c r="W98" t="inlineStr"/>
+      <c r="X98" t="inlineStr">
+        <is>
+          <t>\\DESKTOP-5KNILLM\Users\Usuario\Compartidos\cpim_sistema\dist\Sistema CPIM\trabajos\REGISTRACION\EDSBERG IVAN\CORTES MARIA DANIELLA</t>
         </is>
       </c>
     </row>

</xml_diff>